<commit_message>
First working version of the experiment_controller
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/experiment_controller/Training_Trials.xlsx
+++ b/src/omniroute_operation/src/experiment_controller/Training_Trials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Study\PhD\Training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAF4641-ABFC-4F10-85C8-5F02D23C8A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F257512A-6EA7-44C2-B963-900A73D216D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{83641444-1021-4AA1-B751-AA612C074B23}"/>
   </bookViews>
@@ -59,13 +59,13 @@
     <t>White_Noise</t>
   </si>
   <si>
-    <t>5Khz</t>
-  </si>
-  <si>
     <t>Forced_Choice</t>
   </si>
   <si>
     <t>Choice</t>
+  </si>
+  <si>
+    <t>5KHz</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,7 +454,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -465,10 +465,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -479,10 +479,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -493,15 +493,15 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -510,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -518,13 +518,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -535,10 +535,10 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -546,27 +546,27 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -574,27 +574,27 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -602,13 +602,13 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -619,10 +619,10 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -633,15 +633,15 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
@@ -650,7 +650,7 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -661,10 +661,10 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -672,13 +672,13 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -706,7 +706,7 @@
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -720,7 +720,7 @@
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -734,7 +734,7 @@
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>